<commit_message>
Adds ID and store lookup methods to StoreData
ID looks for the Store ID, given the store name, while store looks for
the Store name given the store ID.

Ammends Menu.xlsx as there was a missing param.
</commit_message>
<xml_diff>
--- a/Menu.xlsx
+++ b/Menu.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9E4E07-803A-48DF-ACD4-06C0D76E4886}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D615CBE0-E398-404F-80FD-99F80CC87C22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="1510" windowWidth="14400" windowHeight="7360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="310" yWindow="1280" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ah Beng Drink" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>Normal,Chino,O,Gao</t>
   </si>
   <si>
-    <t>0.00,0.00,0.00</t>
-  </si>
-  <si>
     <t>A2</t>
   </si>
   <si>
@@ -84,6 +81,9 @@
   </si>
   <si>
     <t>Amount_2</t>
+  </si>
+  <si>
+    <t>0.00,0.00,0.00,0.00</t>
   </si>
 </sst>
 </file>
@@ -410,8 +410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -429,22 +429,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -467,15 +467,15 @@
         <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -490,15 +490,15 @@
         <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -513,10 +513,11 @@
         <v>6</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -525,7 +526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4924435-A4E9-4FBC-873A-6D627DAB6B64}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -542,22 +543,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -565,13 +566,13 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1">
         <v>1.5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
@@ -581,16 +582,16 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>5</v>
@@ -600,16 +601,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Switches Queue to list and restructures Data file
Changes queue to list to store all new orders when initialising bot
data.

Includes new column in Menu.xlsx to categorise items according to type
e.g(western, chinese, drinks, etc).

Adds new attribute self.cat to Menu object. self.cat is another
dataframe containing the categories for each order item. Splits
the code in item and cost and adds new methods such as
from_tuple_to_cost and from_tuple_to_food when needing to convert from
tuple to cost or food respectively. list_of_cat returns the list of
cateogries and cat_subset returns the list of IDs, associated with
the given category.
</commit_message>
<xml_diff>
--- a/Menu.xlsx
+++ b/Menu.xlsx
@@ -1,27 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D615CBE0-E398-404F-80FD-99F80CC87C22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8B7965-898E-4BF7-84BF-878D60CCF9E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="310" yWindow="1280" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ah Beng Drink" sheetId="1" r:id="rId1"/>
-    <sheet name="Ah Lian food" sheetId="2" r:id="rId2"/>
+    <sheet name="Ah Lian Food" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
   <si>
     <t>OrderID</t>
   </si>
@@ -29,9 +37,6 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>A1</t>
-  </si>
-  <si>
     <t>Milo</t>
   </si>
   <si>
@@ -44,15 +49,9 @@
     <t>Normal,Chino,O,Gao</t>
   </si>
   <si>
-    <t>A2</t>
-  </si>
-  <si>
     <t>Kopi</t>
   </si>
   <si>
-    <t>A3</t>
-  </si>
-  <si>
     <t>Teh</t>
   </si>
   <si>
@@ -84,6 +83,21 @@
   </si>
   <si>
     <t>0.00,0.00,0.00,0.00</t>
+  </si>
+  <si>
+    <t>Ice Lemon Tea</t>
+  </si>
+  <si>
+    <t>Drink</t>
+  </si>
+  <si>
+    <t>Cat_1</t>
+  </si>
+  <si>
+    <t>Chinese</t>
+  </si>
+  <si>
+    <t>Western</t>
   </si>
 </sst>
 </file>
@@ -125,9 +139,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,112 +426,125 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G4"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="5.54296875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>1.5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
         <v>17</v>
       </c>
-      <c r="F1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
-        <v>1.5</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="F4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G4" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
+      <c r="H4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -524,99 +555,134 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4924435-A4E9-4FBC-873A-6D627DAB6B64}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.08984375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Adds blocking item feature
Adds new method to block certain items from being selected.
Only a list of items that are available will be returned when
cat_subset and list_of_cats is called.

check_avail checks for the item's availability.

Menu has been slightly tweaked to exclude options with $0.00
</commit_message>
<xml_diff>
--- a/Menu.xlsx
+++ b/Menu.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A8B7965-898E-4BF7-84BF-878D60CCF9E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8A5141-0260-44C4-98E2-B9054C6D9072}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ah Beng Drink" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
   <si>
     <t>OrderID</t>
   </si>
@@ -40,12 +40,6 @@
     <t>Milo</t>
   </si>
   <si>
-    <t>Ice,No Ice</t>
-  </si>
-  <si>
-    <t>0.50,0.00</t>
-  </si>
-  <si>
     <t>Normal,Chino,O,Gao</t>
   </si>
   <si>
@@ -64,9 +58,6 @@
     <t>Fish n' Chips</t>
   </si>
   <si>
-    <t>Chilli,No Chilli</t>
-  </si>
-  <si>
     <t>Item</t>
   </si>
   <si>
@@ -98,6 +89,15 @@
   </si>
   <si>
     <t>Western</t>
+  </si>
+  <si>
+    <t>Ice</t>
+  </si>
+  <si>
+    <t>Chilli</t>
+  </si>
+  <si>
+    <t>0.50</t>
   </si>
 </sst>
 </file>
@@ -144,7 +144,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -428,16 +428,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" customWidth="1"/>
+    <col min="6" max="6" width="9.54296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.453125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.08984375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.453125" bestFit="1" customWidth="1"/>
@@ -448,25 +449,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -474,7 +475,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -483,16 +484,16 @@
         <v>1.5</v>
       </c>
       <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>0.5</v>
+      </c>
+      <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
       <c r="H2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -500,25 +501,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>0.5</v>
+      </c>
+      <c r="G3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" t="s">
-        <v>5</v>
-      </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -526,30 +527,31 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>0.5</v>
+      </c>
+      <c r="G4" t="s">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" t="s">
-        <v>5</v>
-      </c>
       <c r="H4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -557,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4924435-A4E9-4FBC-873A-6D627DAB6B64}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -577,25 +579,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -603,19 +605,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D2" s="1">
         <v>1.5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -625,19 +627,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -647,19 +649,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -669,19 +671,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>